<commit_message>
Implementando a aba da UF
- Adicionei todos os shapefiles do municipios de cada estado
- Implementei o ui e server da aba UF
- Tem muitos erros ainda, principalemente nos bins dos mapas que a função retorna erro quando os dados são mt desbalanceados
</commit_message>
<xml_diff>
--- a/Dashboard/aplicativo/estados_siglas.xlsx
+++ b/Dashboard/aplicativo/estados_siglas.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\covidmetrika\COVID-19\Dashboard\aplicativo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Estado</t>
   </si>
@@ -179,38 +187,41 @@
   </si>
   <si>
     <t>TO</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="OpenSans"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF337AB7"/>
       <name val="OpenSans"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="OpenSans"/>
     </font>
@@ -220,7 +231,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -236,7 +247,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -250,41 +267,37 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -474,273 +487,362 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="C10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="C11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="C12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="C13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="C14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="C15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="C16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="C17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19">
+      <c r="C18">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20">
+      <c r="C19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21">
+      <c r="C20">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22">
+      <c r="C21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23">
+      <c r="C22">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24">
+      <c r="C23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25">
+      <c r="C24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="C25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="C26">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28">
+      <c r="C27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
-    <hyperlink r:id="rId6" ref="A7"/>
-    <hyperlink r:id="rId7" ref="A8"/>
-    <hyperlink r:id="rId8" ref="A9"/>
-    <hyperlink r:id="rId9" ref="A10"/>
-    <hyperlink r:id="rId10" ref="A11"/>
-    <hyperlink r:id="rId11" ref="A12"/>
-    <hyperlink r:id="rId12" ref="A13"/>
-    <hyperlink r:id="rId13" ref="A14"/>
-    <hyperlink r:id="rId14" ref="A15"/>
-    <hyperlink r:id="rId15" ref="A16"/>
-    <hyperlink r:id="rId16" ref="A17"/>
-    <hyperlink r:id="rId17" ref="A18"/>
-    <hyperlink r:id="rId18" ref="A19"/>
-    <hyperlink r:id="rId19" ref="A20"/>
-    <hyperlink r:id="rId20" ref="A21"/>
-    <hyperlink r:id="rId21" ref="A22"/>
-    <hyperlink r:id="rId22" ref="A23"/>
-    <hyperlink r:id="rId23" ref="A24"/>
-    <hyperlink r:id="rId24" ref="A25"/>
-    <hyperlink r:id="rId25" ref="A26"/>
-    <hyperlink r:id="rId26" ref="A27"/>
-    <hyperlink r:id="rId27" ref="A28"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="A23" r:id="rId22"/>
+    <hyperlink ref="A24" r:id="rId23"/>
+    <hyperlink ref="A25" r:id="rId24"/>
+    <hyperlink ref="A26" r:id="rId25"/>
+    <hyperlink ref="A27" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
   </hyperlinks>
-  <drawing r:id="rId28"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>